<commit_message>
PCB stackup info updated
PCB stackup info updated
</commit_message>
<xml_diff>
--- a/mft/pcb/Stackup/WI4B_Wilamp_PCB Stackup.xlsx
+++ b/mft/pcb/Stackup/WI4B_Wilamp_PCB Stackup.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lab_ws\prj\wi4b\Wilamp DCU\Wilamp_DCU_v2.0\mft\pcb\Stackup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="WI4B 4L PCB Stack Up" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -70,30 +75,30 @@
     <t>9-5-9</t>
   </si>
   <si>
-    <t>Wilamp DCU v1.0.GTO
-Wilamp DCU v1.0.GTS</t>
-  </si>
-  <si>
-    <t>Wilamp DCU v1.0.G1</t>
-  </si>
-  <si>
-    <t>Wilamp DCU v1.0.G2</t>
-  </si>
-  <si>
-    <t>Wilamp DCU v1.0.GBL</t>
-  </si>
-  <si>
-    <t>Wilamp DCU v1.0.GBO
-Wilamp DCU v1.0.GBS</t>
-  </si>
-  <si>
-    <t>Wilamp DCU v1.0.GTL</t>
+    <t>Wilamp DCU v2.0.GTO
+Wilamp DCU v2.0.GTS</t>
+  </si>
+  <si>
+    <t>Wilamp DCU v2.0.GTL</t>
+  </si>
+  <si>
+    <t>Wilamp DCU v2.0.G1</t>
+  </si>
+  <si>
+    <t>Wilamp DCU v2.0.G2</t>
+  </si>
+  <si>
+    <t>Wilamp DCU v2.0.GBL</t>
+  </si>
+  <si>
+    <t>Wilamp DCU v2.0.GBO
+Wilamp DCU v2.0.GBS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,7 +445,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -475,7 +480,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -687,7 +692,7 @@
   <dimension ref="C7:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +758,7 @@
         <v>0.7</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I10" s="30" t="s">
         <v>16</v>
@@ -787,7 +792,7 @@
         <v>1.4</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" s="29"/>
     </row>
@@ -819,7 +824,7 @@
         <v>1.4</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I14" s="29"/>
     </row>
@@ -851,7 +856,7 @@
         <v>0.7</v>
       </c>
       <c r="H16" s="35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16" s="29"/>
     </row>
@@ -865,7 +870,7 @@
         <v>0.5</v>
       </c>
       <c r="H17" s="34" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I17" s="27"/>
     </row>

</xml_diff>